<commit_message>
Correct error in ModbusReference.xlsx
</commit_message>
<xml_diff>
--- a/HighLevelDocs/Canary_Integration_Test/ModbusReference.xlsx
+++ b/HighLevelDocs/Canary_Integration_Test/ModbusReference.xlsx
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>Auto/Stop;F Droop On/Off; V Droop On/Off</t>
-  </si>
-  <si>
-    <t>xxxxxxxxxxxxxxx0 = Stop Mode     xxxxxxxxxxxxxxx1 = Auto Mode xxxxxxxxxxxxx1xx = F Droop On xxxxxxxxxxxxx0xx = F Droop Off 1xxxxxxxxxxxxxxx = V Droop Off 0xxxxxxxxxxxxxxx = V Droop Off</t>
   </si>
   <si>
     <t>NG easYgen 3500 (192.168.10.35 : 502)</t>
@@ -226,19 +223,15 @@
   <si>
     <t>Not yet implemented as of 10/14/2016</t>
   </si>
+  <si>
+    <t>xxxxxxxxxxxxxxx0 = Stop Mode     xxxxxxxxxxxxxxx1 = Auto Mode xxxxxxxxxxxxx1xx = F Droop On xxxxxxxxxxxxx0xx = F Droop Off 1xxxxxxxxxxxxxxx = V Droop On 0xxxxxxxxxxxxxxx = V Droop Off</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,20 +295,20 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -337,16 +330,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,7 +651,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +689,7 @@
         <v>29</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -776,7 +769,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>30</v>
@@ -784,7 +777,7 @@
     </row>
     <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="7">
         <v>4</v>
@@ -852,7 +845,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
@@ -947,7 +940,7 @@
         <v>38</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>31</v>
@@ -962,48 +955,48 @@
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2">
         <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="G16" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="13">
         <v>28</v>
       </c>
       <c r="D17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="G17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="H17" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Merged changes from the public github EPHCC and the internal repo. Branching to let someone verify changes before pushing to Github
</commit_message>
<xml_diff>
--- a/HighLevelDocs/Canary_Integration_Test/ModbusReference.xlsx
+++ b/HighLevelDocs/Canary_Integration_Test/ModbusReference.xlsx
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>Auto/Stop;F Droop On/Off; V Droop On/Off</t>
-  </si>
-  <si>
-    <t>xxxxxxxxxxxxxxx0 = Stop Mode     xxxxxxxxxxxxxxx1 = Auto Mode xxxxxxxxxxxxx1xx = F Droop On xxxxxxxxxxxxx0xx = F Droop Off 1xxxxxxxxxxxxxxx = V Droop Off 0xxxxxxxxxxxxxxx = V Droop Off</t>
   </si>
   <si>
     <t>NG easYgen 3500 (192.168.10.35 : 502)</t>
@@ -226,19 +223,15 @@
   <si>
     <t>Not yet implemented as of 10/14/2016</t>
   </si>
+  <si>
+    <t>xxxxxxxxxxxxxxx0 = Stop Mode     xxxxxxxxxxxxxxx1 = Auto Mode xxxxxxxxxxxxx1xx = F Droop On xxxxxxxxxxxxx0xx = F Droop Off 1xxxxxxxxxxxxxxx = V Droop On 0xxxxxxxxxxxxxxx = V Droop Off</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,20 +295,20 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -337,16 +330,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,7 +651,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +689,7 @@
         <v>29</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -776,7 +769,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>30</v>
@@ -784,7 +777,7 @@
     </row>
     <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="7">
         <v>4</v>
@@ -852,7 +845,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
@@ -947,7 +940,7 @@
         <v>38</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>31</v>
@@ -962,48 +955,48 @@
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2">
         <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="G16" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="13">
         <v>28</v>
       </c>
       <c r="D17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="G17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="H17" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>